<commit_message>
Updated test data for Austria after review
</commit_message>
<xml_diff>
--- a/Test Data/Power_Calculation_Max_Values.xlsx
+++ b/Test Data/Power_Calculation_Max_Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7A59E3-CA94-4742-A194-D1EA0367C8A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F6CDBF-7FC8-48EE-B547-059C9AB3CE15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="6" r:id="rId1"/>
@@ -274,9 +274,6 @@
     <t>Netherlands</t>
   </si>
   <si>
-    <t>NGC-3817/T2808</t>
-  </si>
-  <si>
     <t>Austria</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>Denmark</t>
+  </si>
+  <si>
+    <t>NGC-3817/T2361/T2363/T2364</t>
   </si>
 </sst>
 </file>
@@ -2199,6 +2199,366 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6236C8F-30FF-4725-81D3-278CBAE46F16}">
   <dimension ref="A1:U10"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+    <col min="11" max="11" width="31.6640625" customWidth="1"/>
+    <col min="12" max="12" width="33.77734375" customWidth="1"/>
+    <col min="13" max="13" width="33.33203125" customWidth="1"/>
+    <col min="14" max="14" width="36.21875" customWidth="1"/>
+    <col min="15" max="15" width="35.6640625" customWidth="1"/>
+    <col min="16" max="16" width="36.5546875" customWidth="1"/>
+    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="21"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="D5" s="3"/>
+      <c r="E5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>250</v>
+      </c>
+      <c r="R8" s="14">
+        <v>4000</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="T8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>250</v>
+      </c>
+      <c r="R9" s="14">
+        <v>2200</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="T9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>250</v>
+      </c>
+      <c r="R10" s="14">
+        <v>2200</v>
+      </c>
+      <c r="S10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="T10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="U10" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CC510D-51F9-43D9-85E6-FAE45C0CD296}">
+  <dimension ref="A1:U10"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -2236,367 +2596,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="D5" s="3"/>
-      <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="N8" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q8" s="14">
-        <v>250</v>
-      </c>
-      <c r="R8" s="14">
-        <v>4000</v>
-      </c>
-      <c r="S8" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="T8" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="U8" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q9" s="14">
-        <v>250</v>
-      </c>
-      <c r="R9" s="14">
-        <v>2200</v>
-      </c>
-      <c r="S9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="U9" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="O10" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="P10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q10" s="14">
-        <v>250</v>
-      </c>
-      <c r="R10" s="14">
-        <v>2200</v>
-      </c>
-      <c r="S10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="T10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="U10" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CC510D-51F9-43D9-85E6-FAE45C0CD296}">
-  <dimension ref="A1:U10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
-    <col min="11" max="11" width="31.6640625" customWidth="1"/>
-    <col min="12" max="12" width="33.77734375" customWidth="1"/>
-    <col min="13" max="13" width="33.33203125" customWidth="1"/>
-    <col min="14" max="14" width="36.21875" customWidth="1"/>
-    <col min="15" max="15" width="35.6640625" customWidth="1"/>
-    <col min="16" max="16" width="36.5546875" customWidth="1"/>
-    <col min="21" max="21" width="13.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="11" t="s">
@@ -2624,7 +2624,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="4"/>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Updated Norway market Max value sheet
</commit_message>
<xml_diff>
--- a/Test Data/Power_Calculation_Max_Values.xlsx
+++ b/Test Data/Power_Calculation_Max_Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD70390C-9762-4ADE-9372-31D21AFCDD9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDE0FEF-4017-4149-AD16-3C20FBACC6DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="8" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Germany" sheetId="6" r:id="rId1"/>
@@ -303,10 +303,10 @@
     <t>NGC-3104/T3011/T3012/T3013</t>
   </si>
   <si>
-    <t>NGC-2931/T3094</t>
-  </si>
-  <si>
-    <t>NGC-2920/T3128</t>
+    <t>NGC-2931/T3092/T3093/T3094</t>
+  </si>
+  <si>
+    <t>NGC-2920/T3126/T3127/T3128</t>
   </si>
 </sst>
 </file>
@@ -3285,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB7751D-C581-4F2B-AC45-046EAA2B9A26}">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection sqref="A1:V10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4007,14 +4007,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43728AA9-E03B-42C7-A0E2-6147CC4A000D}">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="2" max="2" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" customWidth="1"/>
     <col min="5" max="5" width="16.5546875" customWidth="1"/>
@@ -4371,8 +4371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0363BE-B97C-461D-A985-75E0DCD277BB}">
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>